<commit_message>
Cleaned and read in data from additional trials from systematic review
</commit_message>
<xml_diff>
--- a/new_columns_with_missing_values.xlsx
+++ b/new_columns_with_missing_values.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="100">
   <si>
     <t xml:space="preserve">study</t>
   </si>
@@ -225,6 +225,24 @@
   </si>
   <si>
     <t xml:space="preserve">50% improvement from baseline score</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Forest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fluoxetine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USA, Puerto Rico</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Levomilnacipran (40mg)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Levomilnacipran (80mg)</t>
   </si>
   <si>
     <t xml:space="preserve">Hughes</t>
@@ -1233,45 +1251,61 @@
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
+      <c r="G6" s="2" t="n">
+        <v>61.5</v>
+      </c>
       <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
+      <c r="I6" s="2" t="n">
+        <v>134</v>
+      </c>
+      <c r="J6" s="2" t="n">
+        <v>61.1</v>
+      </c>
       <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
+      <c r="L6" s="2" t="n">
+        <v>140</v>
+      </c>
+      <c r="M6" s="2" t="n">
+        <v>37.13</v>
+      </c>
       <c r="N6" s="2"/>
-      <c r="O6" s="2"/>
-      <c r="P6" s="2"/>
+      <c r="O6" s="2" t="n">
+        <v>112</v>
+      </c>
+      <c r="P6" s="2" t="n">
+        <v>38.2</v>
+      </c>
       <c r="Q6" s="2"/>
-      <c r="R6" s="2"/>
-      <c r="S6" s="2"/>
-      <c r="T6" s="2"/>
-      <c r="U6" s="2"/>
-      <c r="V6" s="2"/>
-      <c r="W6" s="2"/>
-      <c r="X6" s="2"/>
+      <c r="R6" s="2" t="n">
+        <v>118</v>
+      </c>
+      <c r="S6" s="2" t="n">
+        <v>-24.37</v>
+      </c>
+      <c r="T6" s="2" t="n">
+        <v>11.85</v>
+      </c>
+      <c r="U6" s="2" t="n">
+        <v>112</v>
+      </c>
+      <c r="V6" s="2" t="n">
+        <v>-22.9</v>
+      </c>
+      <c r="W6" s="2" t="n">
+        <v>11.84</v>
+      </c>
+      <c r="X6" s="2" t="n">
+        <v>118</v>
+      </c>
       <c r="Y6" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="Z6" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="AA6" s="2" t="n">
-        <v>7</v>
-      </c>
-      <c r="AB6" s="2" t="n">
-        <v>0.571428571428571</v>
-      </c>
-      <c r="AC6" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="AD6" s="2" t="n">
-        <v>5</v>
-      </c>
-      <c r="AE6" s="2" t="n">
-        <v>0.2</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="Z6" s="2"/>
+      <c r="AA6" s="2"/>
+      <c r="AB6" s="2"/>
+      <c r="AC6" s="2"/>
+      <c r="AD6" s="2"/>
+      <c r="AE6" s="2"/>
       <c r="AF6" s="2"/>
       <c r="AG6" s="2"/>
       <c r="AH6" s="2"/>
@@ -1286,18 +1320,34 @@
       <c r="AQ6" s="2"/>
       <c r="AR6" s="2"/>
       <c r="AS6" s="2"/>
-      <c r="AT6" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="AU6" s="2"/>
-      <c r="AV6" s="2"/>
-      <c r="AW6" s="2"/>
-      <c r="AX6" s="2"/>
-      <c r="AY6" s="2"/>
-      <c r="AZ6" s="2"/>
-      <c r="BA6" s="2"/>
-      <c r="BB6" s="2"/>
-      <c r="BC6" s="2"/>
+      <c r="AT6" s="2"/>
+      <c r="AU6" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="AV6" s="2" t="n">
+        <v>14.7</v>
+      </c>
+      <c r="AW6" s="2" t="n">
+        <v>1.67</v>
+      </c>
+      <c r="AX6" s="2" t="n">
+        <v>14.3</v>
+      </c>
+      <c r="AY6" s="2" t="n">
+        <v>1.59</v>
+      </c>
+      <c r="AZ6" s="2" t="n">
+        <v>14.7</v>
+      </c>
+      <c r="BA6" s="2" t="n">
+        <v>1.67</v>
+      </c>
+      <c r="BB6" s="2" t="n">
+        <v>62.7</v>
+      </c>
+      <c r="BC6" s="2" t="n">
+        <v>69.5</v>
+      </c>
       <c r="BD6" s="2"/>
       <c r="BE6" s="2"/>
       <c r="BF6" s="2"/>
@@ -1305,49 +1355,65 @@
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>62</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
+      <c r="G7" s="2" t="n">
+        <v>61.8</v>
+      </c>
       <c r="H7" s="2"/>
       <c r="I7" s="2" t="n">
-        <v>82</v>
-      </c>
-      <c r="J7" s="2"/>
+        <v>134</v>
+      </c>
+      <c r="J7" s="2" t="n">
+        <v>61.1</v>
+      </c>
       <c r="K7" s="2"/>
       <c r="L7" s="2" t="n">
-        <v>44</v>
+        <v>140</v>
       </c>
       <c r="M7" s="2" t="n">
-        <v>35.08</v>
+        <v>38.52</v>
       </c>
       <c r="N7" s="2"/>
       <c r="O7" s="2" t="n">
-        <v>82</v>
+        <v>115</v>
       </c>
       <c r="P7" s="2" t="n">
-        <v>37.24</v>
+        <v>38.2</v>
       </c>
       <c r="Q7" s="2"/>
       <c r="R7" s="2" t="n">
-        <v>44</v>
-      </c>
-      <c r="S7" s="2"/>
-      <c r="T7" s="2"/>
-      <c r="U7" s="2"/>
-      <c r="V7" s="2"/>
-      <c r="W7" s="2"/>
-      <c r="X7" s="2"/>
+        <v>118</v>
+      </c>
+      <c r="S7" s="2" t="n">
+        <v>-23.28</v>
+      </c>
+      <c r="T7" s="2" t="n">
+        <v>11.9</v>
+      </c>
+      <c r="U7" s="2" t="n">
+        <v>115</v>
+      </c>
+      <c r="V7" s="2" t="n">
+        <v>-22.9</v>
+      </c>
+      <c r="W7" s="2" t="n">
+        <v>11.84</v>
+      </c>
+      <c r="X7" s="2" t="n">
+        <v>118</v>
+      </c>
       <c r="Y7" s="2" t="s">
         <v>63</v>
       </c>
@@ -1372,22 +1438,32 @@
       <c r="AR7" s="2"/>
       <c r="AS7" s="2"/>
       <c r="AT7" s="2"/>
-      <c r="AU7" s="2"/>
+      <c r="AU7" s="2" t="s">
+        <v>74</v>
+      </c>
       <c r="AV7" s="2" t="n">
-        <v>12.3</v>
-      </c>
-      <c r="AW7" s="2"/>
+        <v>14.8</v>
+      </c>
+      <c r="AW7" s="2" t="n">
+        <v>1.62</v>
+      </c>
       <c r="AX7" s="2" t="n">
-        <v>12.4</v>
-      </c>
-      <c r="AY7" s="2"/>
-      <c r="AZ7" s="2"/>
-      <c r="BA7" s="2"/>
+        <v>14.3</v>
+      </c>
+      <c r="AY7" s="2" t="n">
+        <v>1.59</v>
+      </c>
+      <c r="AZ7" s="2" t="n">
+        <v>14.7</v>
+      </c>
+      <c r="BA7" s="2" t="n">
+        <v>1.67</v>
+      </c>
       <c r="BB7" s="2" t="n">
-        <v>47.6</v>
+        <v>70.1</v>
       </c>
       <c r="BC7" s="2" t="n">
-        <v>56.8</v>
+        <v>69.5</v>
       </c>
       <c r="BD7" s="2"/>
       <c r="BE7" s="2"/>
@@ -1396,49 +1472,65 @@
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>76</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>77</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>62</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
+      <c r="G8" s="2" t="n">
+        <v>59.4</v>
+      </c>
       <c r="H8" s="2"/>
       <c r="I8" s="2" t="n">
-        <v>88</v>
-      </c>
-      <c r="J8" s="2"/>
+        <v>138</v>
+      </c>
+      <c r="J8" s="2" t="n">
+        <v>61.1</v>
+      </c>
       <c r="K8" s="2"/>
       <c r="L8" s="2" t="n">
-        <v>45</v>
+        <v>140</v>
       </c>
       <c r="M8" s="2" t="n">
-        <v>35.39</v>
+        <v>36.76</v>
       </c>
       <c r="N8" s="2"/>
       <c r="O8" s="2" t="n">
-        <v>82</v>
+        <v>110</v>
       </c>
       <c r="P8" s="2" t="n">
-        <v>38.76</v>
+        <v>38.2</v>
       </c>
       <c r="Q8" s="2"/>
       <c r="R8" s="2" t="n">
-        <v>41</v>
-      </c>
-      <c r="S8" s="2"/>
-      <c r="T8" s="2"/>
-      <c r="U8" s="2"/>
-      <c r="V8" s="2"/>
-      <c r="W8" s="2"/>
-      <c r="X8" s="2"/>
+        <v>118</v>
+      </c>
+      <c r="S8" s="2" t="n">
+        <v>-22.64</v>
+      </c>
+      <c r="T8" s="2" t="n">
+        <v>11.74</v>
+      </c>
+      <c r="U8" s="2" t="n">
+        <v>110</v>
+      </c>
+      <c r="V8" s="2" t="n">
+        <v>-22.9</v>
+      </c>
+      <c r="W8" s="2" t="n">
+        <v>11.84</v>
+      </c>
+      <c r="X8" s="2" t="n">
+        <v>118</v>
+      </c>
       <c r="Y8" s="2" t="s">
         <v>63</v>
       </c>
@@ -1463,22 +1555,32 @@
       <c r="AR8" s="2"/>
       <c r="AS8" s="2"/>
       <c r="AT8" s="2"/>
-      <c r="AU8" s="2"/>
+      <c r="AU8" s="2" t="s">
+        <v>74</v>
+      </c>
       <c r="AV8" s="2" t="n">
-        <v>11.9</v>
-      </c>
-      <c r="AW8" s="2"/>
+        <v>14.8</v>
+      </c>
+      <c r="AW8" s="2" t="n">
+        <v>1.75</v>
+      </c>
       <c r="AX8" s="2" t="n">
-        <v>12.3</v>
-      </c>
-      <c r="AY8" s="2"/>
-      <c r="AZ8" s="2"/>
-      <c r="BA8" s="2"/>
+        <v>14.3</v>
+      </c>
+      <c r="AY8" s="2" t="n">
+        <v>1.59</v>
+      </c>
+      <c r="AZ8" s="2" t="n">
+        <v>14.7</v>
+      </c>
+      <c r="BA8" s="2" t="n">
+        <v>1.67</v>
+      </c>
       <c r="BB8" s="2" t="n">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="BC8" s="2" t="n">
-        <v>50.5</v>
+        <v>69.5</v>
       </c>
       <c r="BD8" s="2"/>
       <c r="BE8" s="2"/>
@@ -1487,13 +1589,13 @@
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>79</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>80</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>62</v>
@@ -1502,49 +1604,43 @@
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
-      <c r="I9" s="2" t="n">
-        <v>29</v>
-      </c>
+      <c r="I9" s="2"/>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
-      <c r="L9" s="2" t="n">
-        <v>27</v>
-      </c>
+      <c r="L9" s="2"/>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
-      <c r="O9" s="2" t="n">
-        <v>29</v>
-      </c>
+      <c r="O9" s="2"/>
       <c r="P9" s="2"/>
       <c r="Q9" s="2"/>
-      <c r="R9" s="2" t="n">
-        <v>27</v>
-      </c>
-      <c r="S9" s="2" t="n">
-        <v>-16.5</v>
-      </c>
-      <c r="T9" s="2" t="n">
-        <v>13.19</v>
-      </c>
-      <c r="U9" s="2" t="n">
-        <v>29</v>
-      </c>
-      <c r="V9" s="2" t="n">
-        <v>-11.9</v>
-      </c>
-      <c r="W9" s="2" t="n">
-        <v>13.2</v>
-      </c>
-      <c r="X9" s="2" t="n">
-        <v>27</v>
-      </c>
-      <c r="Y9" s="2"/>
-      <c r="Z9" s="2"/>
-      <c r="AA9" s="2"/>
-      <c r="AB9" s="2"/>
-      <c r="AC9" s="2"/>
-      <c r="AD9" s="2"/>
-      <c r="AE9" s="2"/>
+      <c r="R9" s="2"/>
+      <c r="S9" s="2"/>
+      <c r="T9" s="2"/>
+      <c r="U9" s="2"/>
+      <c r="V9" s="2"/>
+      <c r="W9" s="2"/>
+      <c r="X9" s="2"/>
+      <c r="Y9" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="Z9" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="AA9" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="AB9" s="2" t="n">
+        <v>0.571428571428571</v>
+      </c>
+      <c r="AC9" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD9" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="AE9" s="2" t="n">
+        <v>0.2</v>
+      </c>
       <c r="AF9" s="2"/>
       <c r="AG9" s="2"/>
       <c r="AH9" s="2"/>
@@ -1559,30 +1655,18 @@
       <c r="AQ9" s="2"/>
       <c r="AR9" s="2"/>
       <c r="AS9" s="2"/>
-      <c r="AT9" s="2"/>
-      <c r="AU9" s="2" t="s">
+      <c r="AT9" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="AV9" s="2" t="n">
-        <v>14.4</v>
-      </c>
-      <c r="AW9" s="2" t="n">
-        <v>1.99</v>
-      </c>
-      <c r="AX9" s="2" t="n">
-        <v>14.8</v>
-      </c>
-      <c r="AY9" s="2" t="n">
-        <v>2.62</v>
-      </c>
+      <c r="AU9" s="2"/>
+      <c r="AV9" s="2"/>
+      <c r="AW9" s="2"/>
+      <c r="AX9" s="2"/>
+      <c r="AY9" s="2"/>
       <c r="AZ9" s="2"/>
       <c r="BA9" s="2"/>
-      <c r="BB9" s="2" t="n">
-        <v>55.2</v>
-      </c>
-      <c r="BC9" s="2" t="n">
-        <v>66.7</v>
-      </c>
+      <c r="BB9" s="2"/>
+      <c r="BC9" s="2"/>
       <c r="BD9" s="2"/>
       <c r="BE9" s="2"/>
       <c r="BF9" s="2"/>
@@ -1593,47 +1677,39 @@
         <v>82</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>84</v>
-      </c>
       <c r="D10" s="2" t="s">
-        <v>85</v>
+        <v>62</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
-      <c r="G10" s="2" t="n">
-        <v>30</v>
-      </c>
-      <c r="H10" s="2" t="n">
-        <v>5.5</v>
-      </c>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
       <c r="I10" s="2" t="n">
-        <v>124</v>
-      </c>
-      <c r="J10" s="2" t="n">
-        <v>30</v>
-      </c>
-      <c r="K10" s="2" t="n">
-        <v>5.5</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
       <c r="L10" s="2" t="n">
-        <v>120</v>
-      </c>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2" t="n">
-        <v>5.5</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="M10" s="2" t="n">
+        <v>35.08</v>
+      </c>
+      <c r="N10" s="2"/>
       <c r="O10" s="2" t="n">
-        <v>79</v>
-      </c>
-      <c r="P10" s="2"/>
-      <c r="Q10" s="2" t="n">
-        <v>5.5</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="P10" s="2" t="n">
+        <v>37.24</v>
+      </c>
+      <c r="Q10" s="2"/>
       <c r="R10" s="2" t="n">
-        <v>74</v>
+        <v>44</v>
       </c>
       <c r="S10" s="2"/>
       <c r="T10" s="2"/>
@@ -1642,18 +1718,14 @@
       <c r="W10" s="2"/>
       <c r="X10" s="2"/>
       <c r="Y10" s="2" t="s">
-        <v>86</v>
+        <v>63</v>
       </c>
       <c r="Z10" s="2"/>
       <c r="AA10" s="2"/>
-      <c r="AB10" s="2" t="n">
-        <v>0.61</v>
-      </c>
+      <c r="AB10" s="2"/>
       <c r="AC10" s="2"/>
       <c r="AD10" s="2"/>
-      <c r="AE10" s="2" t="n">
-        <v>0.59</v>
-      </c>
+      <c r="AE10" s="2"/>
       <c r="AF10" s="2"/>
       <c r="AG10" s="2"/>
       <c r="AH10" s="2"/>
@@ -1669,29 +1741,23 @@
       <c r="AR10" s="2"/>
       <c r="AS10" s="2"/>
       <c r="AT10" s="2"/>
-      <c r="AU10" s="2" t="s">
-        <v>87</v>
-      </c>
+      <c r="AU10" s="2"/>
       <c r="AV10" s="2" t="n">
-        <v>16</v>
-      </c>
-      <c r="AW10" s="2" t="n">
-        <v>1</v>
-      </c>
+        <v>12.3</v>
+      </c>
+      <c r="AW10" s="2"/>
       <c r="AX10" s="2" t="n">
-        <v>16</v>
-      </c>
-      <c r="AY10" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="AZ10" s="2" t="n">
-        <v>16</v>
-      </c>
-      <c r="BA10" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="BB10" s="2"/>
-      <c r="BC10" s="2"/>
+        <v>12.4</v>
+      </c>
+      <c r="AY10" s="2"/>
+      <c r="AZ10" s="2"/>
+      <c r="BA10" s="2"/>
+      <c r="BB10" s="2" t="n">
+        <v>47.6</v>
+      </c>
+      <c r="BC10" s="2" t="n">
+        <v>56.8</v>
+      </c>
       <c r="BD10" s="2"/>
       <c r="BE10" s="2"/>
       <c r="BF10" s="2"/>
@@ -1699,50 +1765,42 @@
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>89</v>
+        <v>65</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>62</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
-      <c r="G11" s="2" t="n">
-        <v>58.8</v>
-      </c>
-      <c r="H11" s="2" t="n">
-        <v>10.9</v>
-      </c>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
       <c r="I11" s="2" t="n">
-        <v>89</v>
-      </c>
-      <c r="J11" s="2" t="n">
-        <v>57.8</v>
-      </c>
-      <c r="K11" s="2" t="n">
-        <v>11.1</v>
-      </c>
+        <v>88</v>
+      </c>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
       <c r="L11" s="2" t="n">
-        <v>85</v>
-      </c>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2" t="n">
-        <v>10.9</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="M11" s="2" t="n">
+        <v>35.39</v>
+      </c>
+      <c r="N11" s="2"/>
       <c r="O11" s="2" t="n">
-        <v>89</v>
-      </c>
-      <c r="P11" s="2"/>
-      <c r="Q11" s="2" t="n">
-        <v>11.1</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="P11" s="2" t="n">
+        <v>38.76</v>
+      </c>
+      <c r="Q11" s="2"/>
       <c r="R11" s="2" t="n">
-        <v>85</v>
+        <v>41</v>
       </c>
       <c r="S11" s="2"/>
       <c r="T11" s="2"/>
@@ -1751,26 +1809,14 @@
       <c r="W11" s="2"/>
       <c r="X11" s="2"/>
       <c r="Y11" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="Z11" s="2" t="n">
-        <v>32</v>
-      </c>
-      <c r="AA11" s="2" t="n">
-        <v>89</v>
-      </c>
-      <c r="AB11" s="2" t="n">
-        <v>0.359550561797753</v>
-      </c>
-      <c r="AC11" s="2" t="n">
-        <v>20</v>
-      </c>
-      <c r="AD11" s="2" t="n">
-        <v>85</v>
-      </c>
-      <c r="AE11" s="2" t="n">
-        <v>0.235294117647059</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="Z11" s="2"/>
+      <c r="AA11" s="2"/>
+      <c r="AB11" s="2"/>
+      <c r="AC11" s="2"/>
+      <c r="AD11" s="2"/>
+      <c r="AE11" s="2"/>
       <c r="AF11" s="2"/>
       <c r="AG11" s="2"/>
       <c r="AH11" s="2"/>
@@ -1785,33 +1831,23 @@
       <c r="AQ11" s="2"/>
       <c r="AR11" s="2"/>
       <c r="AS11" s="2"/>
-      <c r="AT11" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="AU11" s="2" t="s">
-        <v>64</v>
-      </c>
+      <c r="AT11" s="2"/>
+      <c r="AU11" s="2"/>
       <c r="AV11" s="2" t="n">
-        <v>12.1</v>
-      </c>
-      <c r="AW11" s="2" t="n">
-        <v>3.1</v>
-      </c>
+        <v>11.9</v>
+      </c>
+      <c r="AW11" s="2"/>
       <c r="AX11" s="2" t="n">
-        <v>12.1</v>
-      </c>
-      <c r="AY11" s="2" t="n">
-        <v>2.8</v>
-      </c>
-      <c r="AZ11" s="2" t="n">
-        <v>12.1</v>
-      </c>
+        <v>12.3</v>
+      </c>
+      <c r="AY11" s="2"/>
+      <c r="AZ11" s="2"/>
       <c r="BA11" s="2"/>
       <c r="BB11" s="2" t="n">
-        <v>52.8</v>
+        <v>50</v>
       </c>
       <c r="BC11" s="2" t="n">
-        <v>54.1</v>
+        <v>50.5</v>
       </c>
       <c r="BD11" s="2"/>
       <c r="BE11" s="2"/>
@@ -1819,127 +1855,460 @@
       <c r="BG11" s="2"/>
     </row>
     <row r="12">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2" t="n">
+        <v>29</v>
+      </c>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2" t="n">
+        <v>29</v>
+      </c>
+      <c r="P12" s="2"/>
+      <c r="Q12" s="2"/>
+      <c r="R12" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="S12" s="2" t="n">
+        <v>-16.5</v>
+      </c>
+      <c r="T12" s="2" t="n">
+        <v>13.19</v>
+      </c>
+      <c r="U12" s="2" t="n">
+        <v>29</v>
+      </c>
+      <c r="V12" s="2" t="n">
+        <v>-11.9</v>
+      </c>
+      <c r="W12" s="2" t="n">
+        <v>13.2</v>
+      </c>
+      <c r="X12" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="Y12" s="2"/>
+      <c r="Z12" s="2"/>
+      <c r="AA12" s="2"/>
+      <c r="AB12" s="2"/>
+      <c r="AC12" s="2"/>
+      <c r="AD12" s="2"/>
+      <c r="AE12" s="2"/>
+      <c r="AF12" s="2"/>
+      <c r="AG12" s="2"/>
+      <c r="AH12" s="2"/>
+      <c r="AI12" s="2"/>
+      <c r="AJ12" s="2"/>
+      <c r="AK12" s="2"/>
+      <c r="AL12" s="2"/>
+      <c r="AM12" s="2"/>
+      <c r="AN12" s="2"/>
+      <c r="AO12" s="2"/>
+      <c r="AP12" s="2"/>
+      <c r="AQ12" s="2"/>
+      <c r="AR12" s="2"/>
+      <c r="AS12" s="2"/>
+      <c r="AT12" s="2"/>
+      <c r="AU12" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="AV12" s="2" t="n">
+        <v>14.4</v>
+      </c>
+      <c r="AW12" s="2" t="n">
+        <v>1.99</v>
+      </c>
+      <c r="AX12" s="2" t="n">
+        <v>14.8</v>
+      </c>
+      <c r="AY12" s="2" t="n">
+        <v>2.62</v>
+      </c>
+      <c r="AZ12" s="2"/>
+      <c r="BA12" s="2"/>
+      <c r="BB12" s="2" t="n">
+        <v>55.2</v>
+      </c>
+      <c r="BC12" s="2" t="n">
+        <v>66.7</v>
+      </c>
+      <c r="BD12" s="2"/>
+      <c r="BE12" s="2"/>
+      <c r="BF12" s="2"/>
+      <c r="BG12" s="2"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C12" s="3" t="s">
+      <c r="B13" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="H13" s="2" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="I13" s="2" t="n">
+        <v>124</v>
+      </c>
+      <c r="J13" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="K13" s="2" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="L13" s="2" t="n">
+        <v>120</v>
+      </c>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="O13" s="2" t="n">
+        <v>79</v>
+      </c>
+      <c r="P13" s="2"/>
+      <c r="Q13" s="2" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="R13" s="2" t="n">
+        <v>74</v>
+      </c>
+      <c r="S13" s="2"/>
+      <c r="T13" s="2"/>
+      <c r="U13" s="2"/>
+      <c r="V13" s="2"/>
+      <c r="W13" s="2"/>
+      <c r="X13" s="2"/>
+      <c r="Y13" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="Z13" s="2"/>
+      <c r="AA13" s="2"/>
+      <c r="AB13" s="2" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="AC13" s="2"/>
+      <c r="AD13" s="2"/>
+      <c r="AE13" s="2" t="n">
+        <v>0.59</v>
+      </c>
+      <c r="AF13" s="2"/>
+      <c r="AG13" s="2"/>
+      <c r="AH13" s="2"/>
+      <c r="AI13" s="2"/>
+      <c r="AJ13" s="2"/>
+      <c r="AK13" s="2"/>
+      <c r="AL13" s="2"/>
+      <c r="AM13" s="2"/>
+      <c r="AN13" s="2"/>
+      <c r="AO13" s="2"/>
+      <c r="AP13" s="2"/>
+      <c r="AQ13" s="2"/>
+      <c r="AR13" s="2"/>
+      <c r="AS13" s="2"/>
+      <c r="AT13" s="2"/>
+      <c r="AU13" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="AV13" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="AW13" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AX13" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="AY13" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AZ13" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="BA13" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="BB13" s="2"/>
+      <c r="BC13" s="2"/>
+      <c r="BD13" s="2"/>
+      <c r="BE13" s="2"/>
+      <c r="BF13" s="2"/>
+      <c r="BG13" s="2"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3" t="n">
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2" t="n">
+        <v>58.8</v>
+      </c>
+      <c r="H14" s="2" t="n">
+        <v>10.9</v>
+      </c>
+      <c r="I14" s="2" t="n">
+        <v>89</v>
+      </c>
+      <c r="J14" s="2" t="n">
+        <v>57.8</v>
+      </c>
+      <c r="K14" s="2" t="n">
+        <v>11.1</v>
+      </c>
+      <c r="L14" s="2" t="n">
+        <v>85</v>
+      </c>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2" t="n">
+        <v>10.9</v>
+      </c>
+      <c r="O14" s="2" t="n">
+        <v>89</v>
+      </c>
+      <c r="P14" s="2"/>
+      <c r="Q14" s="2" t="n">
+        <v>11.1</v>
+      </c>
+      <c r="R14" s="2" t="n">
+        <v>85</v>
+      </c>
+      <c r="S14" s="2"/>
+      <c r="T14" s="2"/>
+      <c r="U14" s="2"/>
+      <c r="V14" s="2"/>
+      <c r="W14" s="2"/>
+      <c r="X14" s="2"/>
+      <c r="Y14" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="Z14" s="2" t="n">
+        <v>32</v>
+      </c>
+      <c r="AA14" s="2" t="n">
+        <v>89</v>
+      </c>
+      <c r="AB14" s="2" t="n">
+        <v>0.359550561797753</v>
+      </c>
+      <c r="AC14" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="AD14" s="2" t="n">
+        <v>85</v>
+      </c>
+      <c r="AE14" s="2" t="n">
+        <v>0.235294117647059</v>
+      </c>
+      <c r="AF14" s="2"/>
+      <c r="AG14" s="2"/>
+      <c r="AH14" s="2"/>
+      <c r="AI14" s="2"/>
+      <c r="AJ14" s="2"/>
+      <c r="AK14" s="2"/>
+      <c r="AL14" s="2"/>
+      <c r="AM14" s="2"/>
+      <c r="AN14" s="2"/>
+      <c r="AO14" s="2"/>
+      <c r="AP14" s="2"/>
+      <c r="AQ14" s="2"/>
+      <c r="AR14" s="2"/>
+      <c r="AS14" s="2"/>
+      <c r="AT14" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="AU14" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="AV14" s="2" t="n">
+        <v>12.1</v>
+      </c>
+      <c r="AW14" s="2" t="n">
+        <v>3.1</v>
+      </c>
+      <c r="AX14" s="2" t="n">
+        <v>12.1</v>
+      </c>
+      <c r="AY14" s="2" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="AZ14" s="2" t="n">
+        <v>12.1</v>
+      </c>
+      <c r="BA14" s="2"/>
+      <c r="BB14" s="2" t="n">
+        <v>52.8</v>
+      </c>
+      <c r="BC14" s="2" t="n">
+        <v>54.1</v>
+      </c>
+      <c r="BD14" s="2"/>
+      <c r="BE14" s="2"/>
+      <c r="BF14" s="2"/>
+      <c r="BG14" s="2"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3" t="n">
         <v>54.5</v>
       </c>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3" t="n">
+      <c r="H15" s="3"/>
+      <c r="I15" s="3" t="n">
         <v>131</v>
       </c>
-      <c r="J12" s="3" t="n">
+      <c r="J15" s="3" t="n">
         <v>56.6</v>
       </c>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3" t="n">
+      <c r="K15" s="3"/>
+      <c r="L15" s="3" t="n">
         <v>133</v>
       </c>
-      <c r="M12" s="3" t="n">
+      <c r="M15" s="3" t="n">
         <v>32.6</v>
       </c>
-      <c r="N12" s="3"/>
-      <c r="O12" s="3"/>
-      <c r="P12" s="3" t="n">
+      <c r="N15" s="3"/>
+      <c r="O15" s="3"/>
+      <c r="P15" s="3" t="n">
         <v>36.4</v>
       </c>
-      <c r="Q12" s="3"/>
-      <c r="R12" s="3"/>
-      <c r="S12" s="3" t="n">
+      <c r="Q15" s="3"/>
+      <c r="R15" s="3"/>
+      <c r="S15" s="3" t="n">
         <v>-21.9</v>
       </c>
-      <c r="T12" s="3"/>
-      <c r="U12" s="3" t="n">
+      <c r="T15" s="3"/>
+      <c r="U15" s="3" t="n">
         <v>129</v>
       </c>
-      <c r="V12" s="3" t="n">
+      <c r="V15" s="3" t="n">
         <v>-20.2</v>
       </c>
-      <c r="W12" s="3"/>
-      <c r="X12" s="3" t="n">
+      <c r="W15" s="3"/>
+      <c r="X15" s="3" t="n">
         <v>132</v>
       </c>
-      <c r="Y12" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="Z12" s="3" t="n">
+      <c r="Y15" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="Z15" s="3" t="n">
         <v>59</v>
       </c>
-      <c r="AA12" s="3" t="n">
+      <c r="AA15" s="3" t="n">
         <v>129</v>
       </c>
-      <c r="AB12" s="3" t="n">
+      <c r="AB15" s="3" t="n">
         <v>0.457364341085271</v>
       </c>
-      <c r="AC12" s="3" t="n">
+      <c r="AC15" s="3" t="n">
         <v>50</v>
       </c>
-      <c r="AD12" s="3" t="n">
+      <c r="AD15" s="3" t="n">
         <v>132</v>
       </c>
-      <c r="AE12" s="3" t="n">
+      <c r="AE15" s="3" t="n">
         <v>0.378787878787879</v>
       </c>
-      <c r="AF12" s="3"/>
-      <c r="AG12" s="3"/>
-      <c r="AH12" s="3"/>
-      <c r="AI12" s="3"/>
-      <c r="AJ12" s="3"/>
-      <c r="AK12" s="3"/>
-      <c r="AL12" s="3"/>
-      <c r="AM12" s="3"/>
-      <c r="AN12" s="3"/>
-      <c r="AO12" s="3"/>
-      <c r="AP12" s="3"/>
-      <c r="AQ12" s="3"/>
-      <c r="AR12" s="3"/>
-      <c r="AS12" s="3"/>
-      <c r="AT12" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="AU12" s="3" t="s">
+      <c r="AF15" s="3"/>
+      <c r="AG15" s="3"/>
+      <c r="AH15" s="3"/>
+      <c r="AI15" s="3"/>
+      <c r="AJ15" s="3"/>
+      <c r="AK15" s="3"/>
+      <c r="AL15" s="3"/>
+      <c r="AM15" s="3"/>
+      <c r="AN15" s="3"/>
+      <c r="AO15" s="3"/>
+      <c r="AP15" s="3"/>
+      <c r="AQ15" s="3"/>
+      <c r="AR15" s="3"/>
+      <c r="AS15" s="3"/>
+      <c r="AT15" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="AU15" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="AV12" s="3" t="n">
+      <c r="AV15" s="3" t="n">
         <v>12.2</v>
       </c>
-      <c r="AW12" s="3" t="n">
+      <c r="AW15" s="3" t="n">
         <v>2.9</v>
       </c>
-      <c r="AX12" s="3" t="n">
+      <c r="AX15" s="3" t="n">
         <v>12.4</v>
       </c>
-      <c r="AY12" s="3" t="n">
+      <c r="AY15" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="AZ12" s="3" t="n">
+      <c r="AZ15" s="3" t="n">
         <v>12.3</v>
       </c>
-      <c r="BA12" s="3" t="n">
+      <c r="BA15" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="BB12" s="3" t="n">
+      <c r="BB15" s="3" t="n">
         <v>51.9</v>
       </c>
-      <c r="BC12" s="3" t="n">
+      <c r="BC15" s="3" t="n">
         <v>51.9</v>
       </c>
-      <c r="BD12" s="3"/>
-      <c r="BE12" s="3"/>
-      <c r="BF12" s="3"/>
-      <c r="BG12" s="3"/>
+      <c r="BD15" s="3"/>
+      <c r="BE15" s="3"/>
+      <c r="BF15" s="3"/>
+      <c r="BG15" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>